<commit_message>
added carbon source gradient
</commit_message>
<xml_diff>
--- a/data/240808_acetate_glutarate_l-glutamate/240808/combined_metadata.xlsx
+++ b/data/240808_acetate_glutarate_l-glutamate/240808/combined_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,11 +28,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="110">
   <si>
     <t xml:space="preserve">Experimenter's Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Experiment description</t>
+  </si>
+  <si>
     <t xml:space="preserve">Date of Experiment (DD/MM/YY)</t>
   </si>
   <si>
@@ -49,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve">Eric Ulrich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three concentration gradient for measuring v max and Km.</t>
   </si>
   <si>
     <t xml:space="preserve">08.08.2024</t>
@@ -441,7 +447,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -638,16 +644,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="K6:M8 F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="27.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="1" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="27.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="1" width="10.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,25 +675,31 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -709,7 +721,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="K6:M8 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -757,330 +769,330 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1102,7 +1114,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="1" sqref="K6:M8 J9"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1151,258 +1163,258 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1424,7 +1436,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="K6:M8 D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1472,330 +1484,330 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1817,7 +1829,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="1" sqref="K6:M8 J13"/>
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.50390625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1865,130 +1877,130 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2005,130 +2017,130 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2161,8 +2173,8 @@
   </sheetPr>
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6:M8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2210,7 +2222,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>15</v>
@@ -2251,7 +2263,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>7</v>
@@ -2292,7 +2304,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>4</v>
@@ -2333,7 +2345,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2350,7 +2362,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>15</v>
@@ -2392,7 +2404,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>7</v>
@@ -2434,7 +2446,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>4</v>
@@ -2476,7 +2488,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2510,7 +2522,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="K6:M8 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2558,330 +2570,330 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2903,7 +2915,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="1" sqref="K6:M8 J18"/>
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2951,7 +2963,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>0</v>
@@ -2992,7 +3004,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>0</v>
@@ -3033,7 +3045,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>0</v>
@@ -3074,7 +3086,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>0</v>
@@ -3115,7 +3127,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0</v>
@@ -3156,7 +3168,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>0</v>
@@ -3197,7 +3209,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>0</v>
@@ -3238,7 +3250,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>0</v>
@@ -3296,7 +3308,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="1" sqref="K6:M8 K2"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3344,330 +3356,330 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>